<commit_message>
My first push to github for this framework
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="AddUserData" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,12 +21,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
   <si>
     <t xml:space="preserve">admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack Jonson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test@123</t>
   </si>
 </sst>
 </file>
@@ -101,13 +111,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -301,7 +315,7 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -324,4 +338,52 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" display="Test@123"/>
+    <hyperlink ref="F1" r:id="rId2" display="Test@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new teststeps from macbook
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="AddUserData" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="AddPIMUserData" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
@@ -316,7 +317,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -347,11 +348,59 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E1" r:id="rId1" display="Test@123"/>
+    <hyperlink ref="F1" r:id="rId2" display="Test@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">

</xml_diff>

<commit_message>
added new page object model
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
@@ -37,6 +37,30 @@
   </si>
   <si>
     <t xml:space="preserve">Test@123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joseph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mjmartin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sjtodd</t>
   </si>
 </sst>
 </file>
@@ -317,7 +341,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -349,7 +373,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -394,13 +418,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -410,22 +434,62 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>20003</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>2002</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E1" r:id="rId1" display="Test@123"/>
-    <hyperlink ref="F1" r:id="rId2" display="Test@123"/>
+    <hyperlink ref="H1" r:id="rId1" display="Test@123"/>
+    <hyperlink ref="I1" r:id="rId2" display="Test@123"/>
+    <hyperlink ref="H2" r:id="rId3" display="Test@123"/>
+    <hyperlink ref="I2" r:id="rId4" display="Test@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
finally sorted the add user in PIM Module
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t xml:space="preserve">Admin</t>
   </si>
@@ -49,18 +49,6 @@
   </si>
   <si>
     <t xml:space="preserve">mjmartin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Samuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Todd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sjtodd</t>
   </si>
 </sst>
 </file>
@@ -341,7 +329,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="2:2 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -373,7 +361,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="2:2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -418,10 +406,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,7 +431,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="2" t="n">
-        <v>20003</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>8</v>
@@ -452,35 +440,6 @@
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>2002</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -488,8 +447,6 @@
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1" display="Test@123"/>
     <hyperlink ref="I1" r:id="rId2" display="Test@123"/>
-    <hyperlink ref="H2" r:id="rId3" display="Test@123"/>
-    <hyperlink ref="I2" r:id="rId4" display="Test@123"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>